<commit_message>
Extra contorle positie toegevoegd
</commit_message>
<xml_diff>
--- a/stangen/matrix.xlsx
+++ b/stangen/matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maart\Documents\School\Bewegingen\Matlab\Stangenmechanisme\stangen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maart\Desktop\stangen(extrs)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217814C9-6974-4657-BAEA-B665E9FB62AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BFEC22-150C-40B7-BEE5-93207FA487F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17640" yWindow="1308" windowWidth="9576" windowHeight="7176" xr2:uid="{D1FF0060-EEC3-47A8-9826-79EF8CCD87FE}"/>
+    <workbookView minimized="1" xWindow="1548" yWindow="6096" windowWidth="9576" windowHeight="7176" xr2:uid="{D1FF0060-EEC3-47A8-9826-79EF8CCD87FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>2x</t>
   </si>
@@ -130,9 +130,6 @@
     <t>11m</t>
   </si>
   <si>
-    <t>Fp</t>
-  </si>
-  <si>
     <t>cos(phi8-pi/2)</t>
   </si>
   <si>
@@ -385,7 +382,37 @@
     <t>M2</t>
   </si>
   <si>
-    <t>cog11_P_y*cos(phi8-pi/2) - cog11_P_x*sin(phi8-pi/2)</t>
+    <t>12x</t>
+  </si>
+  <si>
+    <t>12y</t>
+  </si>
+  <si>
+    <t>12m</t>
+  </si>
+  <si>
+    <t>cog12_P_y*cos(phi8-pi/2) - cog12_P_x*sin(phi8-pi/2)</t>
+  </si>
+  <si>
+    <t>-cog11_P_y</t>
+  </si>
+  <si>
+    <t>cog11_P_x</t>
+  </si>
+  <si>
+    <t>cog12_P_y</t>
+  </si>
+  <si>
+    <t>-cog12_P_x</t>
+  </si>
+  <si>
+    <t>Fp_x</t>
+  </si>
+  <si>
+    <t>Fp_y</t>
+  </si>
+  <si>
+    <t>Fp_p</t>
   </si>
 </sst>
 </file>
@@ -740,10 +767,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01470959-D89B-46F7-9318-AC6F5BBB2101}">
-  <dimension ref="A1:AE31"/>
+  <dimension ref="A1:AH35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AE11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AH21" sqref="AH21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,102 +798,110 @@
     <col min="28" max="28" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="50.88671875" bestFit="1" customWidth="1"/>
-    <col min="31" max="34" width="3.88671875" customWidth="1"/>
+    <col min="31" max="31" width="3.88671875" customWidth="1"/>
+    <col min="32" max="33" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>40</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>42</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>46</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>48</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>50</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>51</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>52</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>53</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>54</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>55</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>56</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>57</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>58</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>59</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>60</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>61</v>
       </c>
-      <c r="AC1" t="s">
-        <v>62</v>
-      </c>
       <c r="AD1" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="AE1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -952,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1041,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1130,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1219,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1308,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1397,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1486,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1575,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1664,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1753,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1842,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1931,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2020,10 +2058,10 @@
         <v>0</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2112,10 +2150,10 @@
         <v>0</v>
       </c>
       <c r="AD15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2204,7 +2242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2293,7 +2331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2382,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -2471,7 +2509,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -2559,11 +2597,11 @@
       <c r="AC20">
         <v>0</v>
       </c>
-      <c r="AD20" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2651,219 +2689,267 @@
       <c r="AC21">
         <v>1</v>
       </c>
-      <c r="AD21" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AG21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="AE22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="H23" t="s">
         <v>68</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="V23" s="3"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="J24" s="3" t="s">
+      <c r="K24" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="V24" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="V24" s="3" t="s">
+      <c r="W24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="W24" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>11</v>
       </c>
       <c r="J25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="L25" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="M25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="M25" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
       <c r="L26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M26" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="N26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P26" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="N26" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="O26" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="P26" s="3" t="s">
+      <c r="Q26" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Q26" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
       <c r="P27" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q27" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="Q27" s="3" t="s">
+      <c r="R27" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R27" s="3" t="s">
+      <c r="S27" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="S27" s="3" t="s">
+      <c r="T27" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="T27" s="3" t="s">
+      <c r="U27" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="U27" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>20</v>
       </c>
       <c r="R28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="S28" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="S28" s="3" t="s">
+      <c r="V28" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="X28" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="V28" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="W28" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="X28" s="3" t="s">
+      <c r="Y28" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Y28" s="3" t="s">
+      <c r="AD28" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AD28" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AH28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>23</v>
       </c>
       <c r="T29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="U29" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="U29" s="3" t="s">
+      <c r="Z29" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="Z29" s="3" t="s">
+      <c r="AA29" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="AA29" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
       <c r="X30" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y30" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z30" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="Y30" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z30" s="3" t="s">
+      <c r="AA30" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB30" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="AA30" s="3" t="s">
+      <c r="AC30" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AB30" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC30" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="AB31" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="AC31" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD31" s="3" t="s">
+      <c r="AF31" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG31" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF32">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>115</v>
       </c>
+      <c r="AD33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG33">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD34" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG34" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH34">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="AG35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2872,15 +2958,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100371174F9DAA68943A4F64D1C7FA5190F" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5a64f488b7f48387ab5d7e9136d716b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cd9202a6-e211-4275-8e27-b09f1131300c" xmlns:ns4="61dace89-6e26-49db-a801-3b0b4dff7cd3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0afca69b80ee5fa63ea8b88fe6e12985" ns3:_="" ns4:_="">
     <xsd:import namespace="cd9202a6-e211-4275-8e27-b09f1131300c"/>
@@ -3051,6 +3128,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3058,14 +3144,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ADB9C3B-F1A3-47BF-BD63-EC6CB01E6136}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CAEA2EE-DDD0-4F6D-B095-2250A53463BD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3080,6 +3158,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ADB9C3B-F1A3-47BF-BD63-EC6CB01E6136}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>